<commit_message>
Updated PCM playback doc. Implemented __SOUND_TARGET_TIMER_US_PER_INTERRUPT.
</commit_message>
<xml_diff>
--- a/doc/PCM-Playback.xlsx
+++ b/doc/PCM-Playback.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">PCM Playback </t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t xml:space="preserve">Real us/interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efective us/interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfeasible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum acceptable quality</t>
   </si>
 </sst>
 </file>
@@ -49,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,11 +131,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -128,7 +149,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -148,152 +169,243 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B3" s="3" t="n">
+      <c r="A3" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>11025</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">ROUND(A3/B3,0)</f>
+        <v>91</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <f aca="false">C3-66</f>
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">D3+20 * (ROUND(MOD(D3,20)/20,0))-MOD(D3,20)</f>
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <f aca="false">ROUND(A4/B4,0)</f>
+        <v>111</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <f aca="false">C4-66</f>
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">D4+20 * (ROUND(MOD(D4,20)/20,0))-MOD(D4,20)</f>
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>8000</v>
       </c>
-      <c r="C3" s="3" t="n">
-        <f aca="false">ROUND(A3/B3,0)</f>
+      <c r="C5" s="4" t="n">
+        <f aca="false">ROUND(A5/B5,0)</f>
         <v>125</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <f aca="false">C3-66</f>
+      <c r="D5" s="4" t="n">
+        <f aca="false">C5-66</f>
         <v>59</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <f aca="false">B3-1000</f>
+      <c r="E5" s="1" t="n">
+        <f aca="false">D5+20 * (ROUND(MOD(D5,20)/20,0))-MOD(D5,20)</f>
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <f aca="false">B5-1000</f>
         <v>7000</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <f aca="false">ROUND(A4/B4,0)</f>
+      <c r="C6" s="4" t="n">
+        <f aca="false">ROUND(A6/B6,0)</f>
         <v>143</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <f aca="false">C4-66</f>
+      <c r="D6" s="4" t="n">
+        <f aca="false">C6-66</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <f aca="false">B4-1000</f>
+      <c r="E6" s="1" t="n">
+        <f aca="false">D6+20 * (ROUND(MOD(D6,20)/20,0))-MOD(D6,20)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <f aca="false">B6-1000</f>
         <v>6000</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <f aca="false">ROUND(A5/B5,0)</f>
+      <c r="C7" s="4" t="n">
+        <f aca="false">ROUND(A7/B7,0)</f>
         <v>167</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <f aca="false">C5-66</f>
+      <c r="D7" s="4" t="n">
+        <f aca="false">C7-66</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <f aca="false">B5-1000</f>
+      <c r="E7" s="1" t="n">
+        <f aca="false">D7+20 * (ROUND(MOD(D7,20)/20,0))-MOD(D7,20)</f>
+        <v>100</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <f aca="false">B7-1000</f>
         <v>5000</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <f aca="false">ROUND(A6/B6,0)</f>
+      <c r="C8" s="4" t="n">
+        <f aca="false">ROUND(A8/B8,0)</f>
         <v>200</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <f aca="false">C6-66</f>
+      <c r="D8" s="4" t="n">
+        <f aca="false">C8-66</f>
         <v>134</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <f aca="false">B6-1000</f>
+      <c r="E8" s="1" t="n">
+        <f aca="false">D8+20 * (ROUND(MOD(D8,20)/20,0))-MOD(D8,20)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <f aca="false">B8-1000</f>
         <v>4000</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <f aca="false">ROUND(A7/B7,0)</f>
+      <c r="C9" s="4" t="n">
+        <f aca="false">ROUND(A9/B9,0)</f>
         <v>250</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <f aca="false">C7-66</f>
+      <c r="D9" s="4" t="n">
+        <f aca="false">C9-66</f>
         <v>184</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <f aca="false">B7-1000</f>
+      <c r="E9" s="1" t="n">
+        <f aca="false">D9+20 * (ROUND(MOD(D9,20)/20,0))-MOD(D9,20)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <f aca="false">B9-1000</f>
         <v>3000</v>
       </c>
-      <c r="C8" s="3" t="n">
-        <f aca="false">ROUND(A8/B8,0)</f>
+      <c r="C10" s="4" t="n">
+        <f aca="false">ROUND(A10/B10,0)</f>
         <v>333</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <f aca="false">C8-66</f>
+      <c r="D10" s="4" t="n">
+        <f aca="false">C10-66</f>
         <v>267</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B9" s="3" t="n">
-        <f aca="false">B8-1000</f>
+      <c r="E10" s="1" t="n">
+        <f aca="false">D10+20 * (ROUND(MOD(D10,20)/20,0))-MOD(D10,20)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <f aca="false">B10-1000</f>
         <v>2000</v>
       </c>
-      <c r="C9" s="3" t="n">
-        <f aca="false">ROUND(A9/B9,0)</f>
+      <c r="C11" s="4" t="n">
+        <f aca="false">ROUND(A11/B11,0)</f>
         <v>500</v>
       </c>
-      <c r="D9" s="3" t="n">
-        <f aca="false">C9-66</f>
+      <c r="D11" s="4" t="n">
+        <f aca="false">C11-66</f>
         <v>434</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">D11+20 * (ROUND(MOD(D11,20)/20,0))-MOD(D11,20)</f>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated PCM playback doc.
</commit_message>
<xml_diff>
--- a/doc/PCM-Playback.xlsx
+++ b/doc/PCM-Playback.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">PCM Playback </t>
   </si>
@@ -46,7 +46,10 @@
     <t xml:space="preserve">Unfeasible</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum</t>
+    <t xml:space="preserve">Maximum, without animations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achievable</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum acceptable quality</t>
@@ -171,8 +174,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -256,7 +259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>1000000</v>
       </c>
@@ -299,6 +302,9 @@
         <f aca="false">D6+20 * (ROUND(MOD(D6,20)/20,0))-MOD(D6,20)</f>
         <v>80</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -321,7 +327,7 @@
         <v>100</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated PCM plaback doc.
</commit_message>
<xml_diff>
--- a/doc/PCM-Playback.xlsx
+++ b/doc/PCM-Playback.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t xml:space="preserve">PCM Playback </t>
   </si>
@@ -49,7 +49,13 @@
     <t xml:space="preserve">Maximum, without animations.</t>
   </si>
   <si>
-    <t xml:space="preserve">Achievable</t>
+    <t xml:space="preserve">Achievable in very simple scenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realistic target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realistic target with some animations</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum acceptable quality</t>
@@ -175,7 +181,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>1000000</v>
       </c>
@@ -348,10 +354,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>1000000</v>
       </c>
@@ -372,7 +378,7 @@
         <v>80</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,8 +401,8 @@
         <f aca="false">D10+20 * (ROUND(MOD(D10,20)/20,0))-MOD(D10,20)</f>
         <v>100</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
+      <c r="F10" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,20 +410,22 @@
         <v>1000000</v>
       </c>
       <c r="B11" s="4" t="n">
-        <f aca="false">B10-1000</f>
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="C11" s="4" t="n">
         <f aca="false">ROUND(A11/B11,0)</f>
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D11" s="4" t="n">
         <f aca="false">C11-66</f>
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">D11+20 * (ROUND(MOD(D11,20)/20,0))-MOD(D11,20)</f>
-        <v>140</v>
+        <v>120</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,41 +433,45 @@
         <v>1000000</v>
       </c>
       <c r="B12" s="4" t="n">
-        <f aca="false">B11-1000</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">ROUND(A12/B12,0)</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D12" s="4" t="n">
         <f aca="false">C12-66</f>
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">D12+20 * (ROUND(MOD(D12,20)/20,0))-MOD(D12,20)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>140</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>1000000</v>
       </c>
       <c r="B13" s="4" t="n">
-        <f aca="false">B12-1000</f>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">ROUND(A13/B13,0)</f>
-        <v>333</v>
+        <v>222</v>
       </c>
       <c r="D13" s="4" t="n">
         <f aca="false">C13-66</f>
-        <v>267</v>
+        <v>156</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">D13+20 * (ROUND(MOD(D13,20)/20,0))-MOD(D13,20)</f>
-        <v>260</v>
+        <v>160</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,20 +479,22 @@
         <v>1000000</v>
       </c>
       <c r="B14" s="4" t="n">
-        <f aca="false">B13-1000</f>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="C14" s="4" t="n">
         <f aca="false">ROUND(A14/B14,0)</f>
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D14" s="4" t="n">
         <f aca="false">C14-66</f>
-        <v>434</v>
+        <v>184</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">D14+20 * (ROUND(MOD(D14,20)/20,0))-MOD(D14,20)</f>
-        <v>440</v>
+        <v>180</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated PCM playback metrics.
</commit_message>
<xml_diff>
--- a/doc/PCM-Playback.xlsx
+++ b/doc/PCM-Playback.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">PCM Playback </t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Unfeasible</t>
   </si>
   <si>
+    <t xml:space="preserve">Maximum, with an empty stage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximum, without animations.</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Minimum acceptable quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sounds very bad</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -239,15 +245,15 @@
         <v>23</v>
       </c>
       <c r="D3" s="2" t="n">
-        <f aca="false">C3-66</f>
-        <v>-43</v>
+        <f aca="false">C3-48</f>
+        <v>-25</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">D3+20 * (ROUND(MOD(D3,20)/20,0))-MOD(D3,20)</f>
-        <v>-40</v>
+        <v>-20</v>
       </c>
       <c r="F3" s="2" t="n">
-        <f aca="false">ROUND(A3/(D3+66),0)</f>
+        <f aca="false">ROUND(A3/(D3+48),0)</f>
         <v>43478</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -266,15 +272,15 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="n">
-        <f aca="false">C4-66</f>
-        <v>-24</v>
+        <f aca="false">C4-48</f>
+        <v>-6</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">D4+20 * (ROUND(MOD(D4,20)/20,0))-MOD(D4,20)</f>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <f aca="false">ROUND(A4/(D4+66),0)</f>
+        <f aca="false">ROUND(A4/(D4+48),0)</f>
         <v>23810</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -293,15 +299,15 @@
         <v>63</v>
       </c>
       <c r="D5" s="2" t="n">
-        <f aca="false">C5-66</f>
-        <v>-3</v>
+        <f aca="false">C5-48</f>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">D5+20 * (ROUND(MOD(D5,20)/20,0))-MOD(D5,20)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="n">
-        <f aca="false">ROUND(A5/(D5+66),0)</f>
+        <f aca="false">ROUND(A5/(D5+48),0)</f>
         <v>15873</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -320,22 +326,22 @@
         <v>91</v>
       </c>
       <c r="D6" s="2" t="n">
-        <f aca="false">C6-66</f>
-        <v>25</v>
+        <f aca="false">C6-48</f>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">D6+20 * (ROUND(MOD(D6,20)/20,0))-MOD(D6,20)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="n">
-        <f aca="false">ROUND(A6/(D6+66),0)</f>
+        <f aca="false">ROUND(A6/(D6+48),0)</f>
         <v>10989</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>1000000</v>
       </c>
@@ -347,22 +353,22 @@
         <v>111</v>
       </c>
       <c r="D7" s="2" t="n">
-        <f aca="false">C7-66</f>
-        <v>45</v>
+        <f aca="false">C7-48</f>
+        <v>63</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">D7+20 * (ROUND(MOD(D7,20)/20,0))-MOD(D7,20)</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F7" s="2" t="n">
-        <f aca="false">ROUND(A7/(D7+66),0)</f>
+        <f aca="false">ROUND(A7/(D7+48),0)</f>
         <v>9009</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>1000000</v>
       </c>
@@ -374,22 +380,22 @@
         <v>125</v>
       </c>
       <c r="D8" s="2" t="n">
-        <f aca="false">C8-66</f>
-        <v>59</v>
+        <f aca="false">C8-48</f>
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">D8+20 * (ROUND(MOD(D8,20)/20,0))-MOD(D8,20)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F8" s="2" t="n">
-        <f aca="false">ROUND(A8/(D8+66),0)</f>
+        <f aca="false">ROUND(A8/(D8+48),0)</f>
         <v>8000</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>1000000</v>
       </c>
@@ -402,19 +408,19 @@
         <v>143</v>
       </c>
       <c r="D9" s="2" t="n">
-        <f aca="false">C9-66</f>
-        <v>77</v>
+        <f aca="false">C9-48</f>
+        <v>95</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">D9+20 * (ROUND(MOD(D9,20)/20,0))-MOD(D9,20)</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="n">
-        <f aca="false">ROUND(A9/(D9+66),0)</f>
+        <f aca="false">ROUND(A9/(D9+48),0)</f>
         <v>6993</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,19 +436,19 @@
         <v>167</v>
       </c>
       <c r="D10" s="2" t="n">
-        <f aca="false">C10-66</f>
-        <v>101</v>
+        <f aca="false">C10-48</f>
+        <v>119</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="false">D10+20 * (ROUND(MOD(D10,20)/20,0))-MOD(D10,20)</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F10" s="2" t="n">
-        <f aca="false">ROUND(A10/(D10+66),0)</f>
+        <f aca="false">ROUND(A10/(D10+48),0)</f>
         <v>5988</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,22 +463,22 @@
         <v>182</v>
       </c>
       <c r="D11" s="2" t="n">
-        <f aca="false">C11-66</f>
-        <v>116</v>
+        <f aca="false">C11-48</f>
+        <v>134</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">D11+20 * (ROUND(MOD(D11,20)/20,0))-MOD(D11,20)</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="n">
-        <f aca="false">ROUND(A11/(D11+66),0)</f>
+        <f aca="false">ROUND(A11/(D11+48),0)</f>
         <v>5495</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>1000000</v>
       </c>
@@ -484,22 +490,22 @@
         <v>200</v>
       </c>
       <c r="D12" s="2" t="n">
-        <f aca="false">C12-66</f>
-        <v>134</v>
+        <f aca="false">C12-48</f>
+        <v>152</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">D12+20 * (ROUND(MOD(D12,20)/20,0))-MOD(D12,20)</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="F12" s="2" t="n">
-        <f aca="false">ROUND(A12/(D12+66),0)</f>
+        <f aca="false">ROUND(A12/(D12+48),0)</f>
         <v>5000</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>1000000</v>
       </c>
@@ -511,19 +517,19 @@
         <v>222</v>
       </c>
       <c r="D13" s="2" t="n">
-        <f aca="false">C13-66</f>
-        <v>156</v>
+        <f aca="false">C13-48</f>
+        <v>174</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">D13+20 * (ROUND(MOD(D13,20)/20,0))-MOD(D13,20)</f>
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F13" s="2" t="n">
-        <f aca="false">ROUND(A13/(D13+66),0)</f>
+        <f aca="false">ROUND(A13/(D13+48),0)</f>
         <v>4505</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,19 +544,19 @@
         <v>250</v>
       </c>
       <c r="D14" s="2" t="n">
-        <f aca="false">C14-66</f>
-        <v>184</v>
+        <f aca="false">C14-48</f>
+        <v>202</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">D14+20 * (ROUND(MOD(D14,20)/20,0))-MOD(D14,20)</f>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F14" s="2" t="n">
-        <f aca="false">ROUND(A14/(D14+66),0)</f>
+        <f aca="false">ROUND(A14/(D14+48),0)</f>
         <v>4000</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>